<commit_message>
compile and package 1.1.2
</commit_message>
<xml_diff>
--- a/tools_scripts/CharactorTable_template.xlsx
+++ b/tools_scripts/CharactorTable_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\TRPG-Replay-Generator\tools_scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E103DA24-E580-4B37-84B6-EA0B595B2104}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{061D1D42-9F6E-4C45-B21E-254E0EEE374D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="150" yWindow="1965" windowWidth="16710" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="角色配置" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="741" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="742" uniqueCount="288">
   <si>
     <t>Name</t>
   </si>
@@ -917,6 +917,10 @@
   </si>
   <si>
     <t>标准女声</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NA</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1086,7 +1090,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1843,10 +1847,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{166DC2E1-0816-49B8-A2B0-16702A9B6229}">
-  <dimension ref="A1:A93"/>
+  <dimension ref="A1:A94"/>
   <sheetViews>
-    <sheetView topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="A80" sqref="A80"/>
+    <sheetView topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="A95" sqref="A95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2410,6 +2414,11 @@
       <c r="A93" t="str">
         <f>Azure普通话音源!G14</f>
         <v>Azure::zh-CN-YunyeNeural</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>287</v>
       </c>
     </row>
   </sheetData>

</xml_diff>